<commit_message>
Update the utilities and mIOU
</commit_message>
<xml_diff>
--- a/Performance_summary.xlsx
+++ b/Performance_summary.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adi\Documents\FourthBrain\CapstoneProject\GitRep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463A33A0-D6EF-4F1A-8EFA-F64834FC3440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D82E85A-B2C2-4DA7-8B69-9F0C9B4987E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{621688BF-A2F8-440F-B3A4-D9921E158F04}"/>
+    <workbookView xWindow="51252" yWindow="2388" windowWidth="19980" windowHeight="13644" activeTab="1" xr2:uid="{621688BF-A2F8-440F-B3A4-D9921E158F04}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="run1" sheetId="1" r:id="rId1"/>
+    <sheet name="run2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>SOTA model</t>
   </si>
@@ -74,6 +75,36 @@
   <si>
     <t>lite-model_deeplabv3-mobilenetv2-int8_1_default_1.tflite</t>
   </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>only 50 images</t>
+  </si>
+  <si>
+    <t>lite-model_deeplabv3-mobilenetv2-int8</t>
+  </si>
+  <si>
+    <t>lite-model_deeplabv3-mobilenetv2-float16</t>
+  </si>
+  <si>
+    <t>lite-model_deeplabv3-mobilenetv2</t>
+  </si>
+  <si>
+    <t>lite-model_mobilenetv2-coco_dr</t>
+  </si>
+  <si>
+    <t>lite-model_deeplabv3-mobilenetv2_dm05</t>
+  </si>
+  <si>
+    <t>lite-model_mobilenetv2-dm05-coco_dr</t>
+  </si>
+  <si>
+    <t>lite-model_deeplabv3-mobilenetv2_dm05-float16</t>
+  </si>
+  <si>
+    <t>lite-model_deeplabv3-mobilenetv2_dm05-int8</t>
+  </si>
 </sst>
 </file>
 
@@ -99,15 +130,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -250,11 +287,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -283,6 +397,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -337,7 +486,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>'run1'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -652,7 +801,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>'run1'!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
@@ -679,7 +828,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>'run1'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
@@ -991,7 +1140,825 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14570544970371407"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.81740557349294063"/>
+          <c:h val="0.7712809857101196"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'run2'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean IOU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.5671866621511027E-2"/>
+                  <c:y val="-4.6296296296296294E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>deeplabv3-mobilenetv2-float16</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.45522222222222219"/>
+                      <c:h val="6.4606663750364543E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-EB14-4FF2-B7BD-B6D0B939C7AC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.3385191770383546E-2"/>
+                  <c:y val="7.8703885972586762E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>deeplabv3-mobilenetv2</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.28994175627240143"/>
+                      <c:h val="0.14953703703703702"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-EB14-4FF2-B7BD-B6D0B939C7AC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9444444444444445E-2"/>
+                  <c:y val="0.23148148148148148"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>mobilenetv2-coco_dr</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-EB14-4FF2-B7BD-B6D0B939C7AC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.31693530748172616"/>
+                  <c:y val="0.30311315252260135"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>deeplabv3-mobilenetv2_dm05</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.23927182993254875"/>
+                      <c:h val="0.16645851560221639"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-EB14-4FF2-B7BD-B6D0B939C7AC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0304659498207804E-2"/>
+                  <c:y val="0.30092592592592593"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>mobilenetv2-dm05-coco</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-EB14-4FF2-B7BD-B6D0B939C7AC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.0536677305239525E-3"/>
+                  <c:y val="-6.7647866485545646E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>deeplabv3-mobilenetv2_dm05-float16</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.2344816733111727"/>
+                      <c:h val="0.2295145128265634"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-EB14-4FF2-B7BD-B6D0B939C7AC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.9089978759667579E-2"/>
+                  <c:y val="-0.12848777172068812"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>deeplabv3-mobilenetv2_dm05-int8</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-EB14-4FF2-B7BD-B6D0B939C7AC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.6164874551971323E-2"/>
+                  <c:y val="-9.2592592592593437E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>deeplabv3-mobilenetv2-int8</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.20687724014336917"/>
+                      <c:h val="0.21597222222222223"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-EB14-4FF2-B7BD-B6D0B939C7AC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'run2'!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.3815182884748003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.36425810904071E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7872118702553401E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6123971014492602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6013846100758999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6256441683919798</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6409571428571401</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0828571428571402E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'run2'!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.692960997509948</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.691463851127606</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.691463851127606</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67300382485835597</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67300382485835597</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.67222259429671005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32988604834797403</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.37975626484471903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-EB14-4FF2-B7BD-B6D0B939C7AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1273967920"/>
+        <c:axId val="1273970832"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1273967920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Mean Inference Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1273970832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1273970832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.30000000000000004"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Mean IOU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1273967920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1547,6 +2514,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1572,6 +3055,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>78104</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FBAD85F-E663-4EC3-9DF1-FBFFBF4BE677}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1887,7 +3413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC8BE79-6642-4C8E-8981-B3DCF56A0DC1}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
@@ -2005,4 +3531,141 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9EE0D2-267C-45F0-8278-8886A7F4C834}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="51.26171875" customWidth="1"/>
+    <col min="2" max="2" width="22.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.41796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="17">
+        <v>3.3815182884748003E-2</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0.692960997509948</v>
+      </c>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="17">
+        <v>5.36425810904071E-2</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0.691463851127606</v>
+      </c>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="17">
+        <v>3.7872118702553401E-2</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0.691463851127606</v>
+      </c>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="17">
+        <v>3.6123971014492602</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0.67300382485835597</v>
+      </c>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="17">
+        <v>3.6013846100758999</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0.67300382485835597</v>
+      </c>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="17">
+        <v>3.6256441683919798</v>
+      </c>
+      <c r="C7" s="15">
+        <v>0.67222259429671005</v>
+      </c>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="23">
+        <v>3.6409571428571401</v>
+      </c>
+      <c r="C8" s="24">
+        <v>0.32988604834797403</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="21">
+        <v>4.0828571428571402E-2</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0.37975626484471903</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>